<commit_message>
includes an is control column
</commit_message>
<xml_diff>
--- a/data/Content_map.xlsx
+++ b/data/Content_map.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="127">
   <si>
     <t>Well</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>H9</t>
+  </si>
+  <si>
+    <t>IsControl</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -467,8 +470,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -488,20 +493,25 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -833,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H85" sqref="H85"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -859,6 +869,9 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
@@ -870,7 +883,9 @@
       <c r="C2" s="1"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="1"/>
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -885,7 +900,9 @@
       <c r="C3" s="1"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -900,7 +917,9 @@
       <c r="C4" s="1"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1017,7 +1036,9 @@
       <c r="C11" s="1"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
       <c r="G11" s="3"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1032,7 +1053,9 @@
       <c r="C12" s="1"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
       <c r="G12" s="3"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1047,7 +1070,9 @@
       <c r="C13" s="1"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="7">
+        <v>1</v>
+      </c>
       <c r="G13" s="3"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -2562,7 +2587,9 @@
       <c r="C86" s="1"/>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
-      <c r="F86" s="1"/>
+      <c r="F86" s="7">
+        <v>1</v>
+      </c>
       <c r="G86" s="3"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
@@ -2577,7 +2604,9 @@
       <c r="C87" s="1"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
-      <c r="F87" s="1"/>
+      <c r="F87" s="7">
+        <v>1</v>
+      </c>
       <c r="G87" s="3"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
@@ -2592,7 +2621,9 @@
       <c r="C88" s="1"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
-      <c r="F88" s="1"/>
+      <c r="F88" s="7">
+        <v>1</v>
+      </c>
       <c r="G88" s="3"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
@@ -2733,7 +2764,9 @@
       <c r="C95" s="1"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
-      <c r="F95" s="1"/>
+      <c r="F95" s="7">
+        <v>1</v>
+      </c>
       <c r="G95" s="3"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
@@ -2748,7 +2781,9 @@
       <c r="C96" s="1"/>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
-      <c r="F96" s="1"/>
+      <c r="F96" s="7">
+        <v>1</v>
+      </c>
       <c r="G96" s="3"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
@@ -2763,7 +2798,9 @@
       <c r="C97" s="1"/>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
-      <c r="F97" s="1"/>
+      <c r="F97" s="7">
+        <v>1</v>
+      </c>
       <c r="G97" s="3"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>

</xml_diff>

<commit_message>
changes to contents maps fixes
stopped adding controls to contents.name
</commit_message>
<xml_diff>
--- a/data/Content_map.xlsx
+++ b/data/Content_map.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="122">
   <si>
     <t>Well</t>
   </si>
@@ -153,24 +153,6 @@
     <t>Protein as supplied</t>
   </si>
   <si>
-    <t>H04</t>
-  </si>
-  <si>
-    <t>H05</t>
-  </si>
-  <si>
-    <t>H06</t>
-  </si>
-  <si>
-    <t>H07</t>
-  </si>
-  <si>
-    <t>H08</t>
-  </si>
-  <si>
-    <t>H09</t>
-  </si>
-  <si>
     <t>H10</t>
   </si>
   <si>
@@ -400,6 +382,9 @@
   </si>
   <si>
     <t>IsControl</t>
+  </si>
+  <si>
+    <t>CHES</t>
   </si>
 </sst>
 </file>
@@ -456,8 +441,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -497,7 +484,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -505,6 +492,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -512,6 +500,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -843,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -870,12 +859,12 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -892,7 +881,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -909,7 +898,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -926,7 +915,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>6</v>
@@ -943,7 +932,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
@@ -960,7 +949,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>6</v>
@@ -977,7 +966,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>6</v>
@@ -994,7 +983,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>6</v>
@@ -1011,7 +1000,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>6</v>
@@ -1079,7 +1068,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
@@ -1098,7 +1087,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -1117,7 +1106,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
@@ -1136,7 +1125,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
@@ -1155,7 +1144,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
@@ -1174,7 +1163,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
@@ -1193,7 +1182,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>14</v>
@@ -1214,7 +1203,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
@@ -1235,7 +1224,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>14</v>
@@ -1319,7 +1308,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>18</v>
@@ -1340,7 +1329,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>18</v>
@@ -1361,7 +1350,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>18</v>
@@ -1382,7 +1371,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>18</v>
@@ -1403,7 +1392,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>18</v>
@@ -1424,7 +1413,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>18</v>
@@ -1445,7 +1434,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>19</v>
@@ -1466,7 +1455,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>19</v>
@@ -1487,7 +1476,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>19</v>
@@ -1571,7 +1560,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>23</v>
@@ -1592,7 +1581,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>23</v>
@@ -1613,7 +1602,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>23</v>
@@ -1634,7 +1623,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>23</v>
@@ -1655,7 +1644,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>23</v>
@@ -1676,7 +1665,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>23</v>
@@ -1697,7 +1686,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>24</v>
@@ -1718,7 +1707,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>24</v>
@@ -1739,7 +1728,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>24</v>
@@ -1823,7 +1812,7 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>28</v>
@@ -1844,7 +1833,7 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>28</v>
@@ -1865,7 +1854,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>28</v>
@@ -1886,7 +1875,7 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>28</v>
@@ -1907,7 +1896,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>28</v>
@@ -1928,7 +1917,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>28</v>
@@ -1949,7 +1938,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>29</v>
@@ -1970,7 +1959,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>29</v>
@@ -1991,7 +1980,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>29</v>
@@ -2075,7 +2064,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>33</v>
@@ -2096,7 +2085,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>33</v>
@@ -2117,7 +2106,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>33</v>
@@ -2138,7 +2127,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>33</v>
@@ -2159,7 +2148,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>33</v>
@@ -2180,7 +2169,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>33</v>
@@ -2201,7 +2190,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>34</v>
@@ -2222,7 +2211,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>34</v>
@@ -2243,7 +2232,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>34</v>
@@ -2327,7 +2316,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>38</v>
@@ -2348,7 +2337,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>38</v>
@@ -2369,7 +2358,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>38</v>
@@ -2390,7 +2379,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>38</v>
@@ -2411,7 +2400,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>38</v>
@@ -2432,7 +2421,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>38</v>
@@ -2453,7 +2442,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>39</v>
@@ -2474,7 +2463,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>39</v>
@@ -2495,7 +2484,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>39</v>
@@ -2579,7 +2568,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>43</v>
@@ -2596,7 +2585,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>43</v>
@@ -2613,7 +2602,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>43</v>
@@ -2630,10 +2619,10 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>44</v>
+        <v>121</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>7</v>
@@ -2651,10 +2640,10 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>7</v>
@@ -2672,10 +2661,10 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>7</v>
@@ -2693,10 +2682,10 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>8</v>
@@ -2714,10 +2703,10 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>8</v>
@@ -2735,10 +2724,10 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>8</v>
@@ -2756,10 +2745,10 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="4"/>
@@ -2773,10 +2762,10 @@
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="4"/>
@@ -2790,10 +2779,10 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="4"/>

</xml_diff>

<commit_message>
changed column names and added decriptionfile
</commit_message>
<xml_diff>
--- a/data/Content_map.xlsx
+++ b/data/Content_map.xlsx
@@ -24,18 +24,9 @@
     <t>Well</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Salt</t>
-  </si>
-  <si>
     <t>pH</t>
   </si>
   <si>
-    <t>d(pKa)/dT</t>
-  </si>
-  <si>
     <t>Lysozyme</t>
   </si>
   <si>
@@ -385,6 +376,15 @@
   </si>
   <si>
     <t>CHES</t>
+  </si>
+  <si>
+    <t>d(pH)/dT</t>
+  </si>
+  <si>
+    <t>Condition Variable 1</t>
+  </si>
+  <si>
+    <t>Condition Varable 2</t>
   </si>
 </sst>
 </file>
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -847,27 +847,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
       <c r="F1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="4"/>
@@ -881,10 +881,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="4"/>
@@ -898,10 +898,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="4"/>
@@ -915,13 +915,13 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -932,13 +932,13 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -949,13 +949,13 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -966,13 +966,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -983,13 +983,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1017,10 +1017,10 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="4"/>
@@ -1034,10 +1034,10 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="4"/>
@@ -1051,10 +1051,10 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="4"/>
@@ -1068,13 +1068,13 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D14" s="4">
         <v>5</v>
@@ -1087,13 +1087,13 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D15" s="4">
         <v>5</v>
@@ -1106,13 +1106,13 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D16" s="4">
         <v>5</v>
@@ -1125,13 +1125,13 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D17" s="4">
         <v>5</v>
@@ -1144,13 +1144,13 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D18" s="4">
         <v>5</v>
@@ -1163,13 +1163,13 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D19" s="4">
         <v>5</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D20" s="4">
         <v>5.5</v>
@@ -1203,13 +1203,13 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D21" s="4">
         <v>5.5</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D22" s="4">
         <v>5.5</v>
@@ -1245,13 +1245,13 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D23" s="4">
         <v>5.5</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D24" s="4">
         <v>5.5</v>
@@ -1287,13 +1287,13 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D25" s="4">
         <v>5.5</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D26" s="4">
         <v>6</v>
@@ -1329,13 +1329,13 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D27" s="4">
         <v>6</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D28" s="4">
         <v>6</v>
@@ -1371,13 +1371,13 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D29" s="4">
         <v>6</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D30" s="4">
         <v>6</v>
@@ -1413,13 +1413,13 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D31" s="4">
         <v>6</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D32" s="4">
         <v>6</v>
@@ -1455,13 +1455,13 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D33" s="4">
         <v>6</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D34" s="4">
         <v>6</v>
@@ -1497,13 +1497,13 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D35" s="4">
         <v>6</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D36" s="4">
         <v>6</v>
@@ -1539,13 +1539,13 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D37" s="4">
         <v>6</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D38" s="4">
         <v>6.5</v>
@@ -1581,13 +1581,13 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D39" s="4">
         <v>6.5</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D40" s="4">
         <v>6.5</v>
@@ -1623,13 +1623,13 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D41" s="4">
         <v>6.5</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D42" s="4">
         <v>6.5</v>
@@ -1665,13 +1665,13 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D43" s="4">
         <v>6.5</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D44" s="4">
         <v>6.5</v>
@@ -1707,13 +1707,13 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D45" s="4">
         <v>6.5</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D46" s="4">
         <v>6.5</v>
@@ -1749,13 +1749,13 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D47" s="4">
         <v>6.5</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D48" s="4">
         <v>6.5</v>
@@ -1791,13 +1791,13 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D49" s="4">
         <v>6.5</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D50" s="4">
         <v>7</v>
@@ -1833,13 +1833,13 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D51" s="4">
         <v>7</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D52" s="4">
         <v>7</v>
@@ -1875,13 +1875,13 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D53" s="4">
         <v>7</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D54" s="4">
         <v>7</v>
@@ -1917,13 +1917,13 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D55" s="4">
         <v>7</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D56" s="4">
         <v>7</v>
@@ -1959,13 +1959,13 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D57" s="4">
         <v>7</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D58" s="4">
         <v>7</v>
@@ -2001,13 +2001,13 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D59" s="4">
         <v>7</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D60" s="4">
         <v>7</v>
@@ -2043,13 +2043,13 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D61" s="4">
         <v>7</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D62" s="4">
         <v>7.5</v>
@@ -2085,13 +2085,13 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D63" s="4">
         <v>7.5</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D64" s="4">
         <v>7.5</v>
@@ -2127,13 +2127,13 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D65" s="4">
         <v>7.5</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D66" s="4">
         <v>7.5</v>
@@ -2169,13 +2169,13 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D67" s="4">
         <v>7.5</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D68" s="4">
         <v>7.5</v>
@@ -2211,13 +2211,13 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D69" s="4">
         <v>7.5</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D70" s="4">
         <v>7.5</v>
@@ -2253,13 +2253,13 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D71" s="4">
         <v>7.5</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D72" s="4">
         <v>7.5</v>
@@ -2295,13 +2295,13 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D73" s="4">
         <v>7.5</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D74" s="4">
         <v>8</v>
@@ -2337,13 +2337,13 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D75" s="4">
         <v>8</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D76" s="4">
         <v>8</v>
@@ -2379,13 +2379,13 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D77" s="4">
         <v>8</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D78" s="4">
         <v>8</v>
@@ -2421,13 +2421,13 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D79" s="4">
         <v>8</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D80" s="4">
         <v>8.5</v>
@@ -2463,13 +2463,13 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D81" s="4">
         <v>8.5</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D82" s="4">
         <v>8.5</v>
@@ -2505,13 +2505,13 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D83" s="4">
         <v>8.5</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D84" s="4">
         <v>8.5</v>
@@ -2547,13 +2547,13 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D85" s="4">
         <v>8.5</v>
@@ -2568,10 +2568,10 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="4"/>
@@ -2585,10 +2585,10 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="4"/>
@@ -2602,10 +2602,10 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="4"/>
@@ -2619,13 +2619,13 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D89" s="4">
         <v>9</v>
@@ -2640,13 +2640,13 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D90" s="4">
         <v>9</v>
@@ -2661,13 +2661,13 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D91" s="4">
         <v>9</v>
@@ -2682,13 +2682,13 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D92" s="4">
         <v>9</v>
@@ -2703,13 +2703,13 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="C93" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D93" s="4">
         <v>9</v>
@@ -2724,13 +2724,13 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D94" s="4">
         <v>9</v>
@@ -2745,10 +2745,10 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="4"/>
@@ -2762,10 +2762,10 @@
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="4"/>
@@ -2779,10 +2779,10 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="4"/>

</xml_diff>

<commit_message>
meltdown now reads in tab delimited text files
</commit_message>
<xml_diff>
--- a/data/Content_map.xlsx
+++ b/data/Content_map.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,22 +390,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.00;\-###0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8.25"/>
-      <name val="Microsoft Sans Serif"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -419,6 +414,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -443,44 +444,42 @@
   </borders>
   <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -829,365 +828,367 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="1" max="1" width="11" style="2"/>
+    <col min="2" max="2" width="19" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <v>1</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>1</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>1</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <v>1</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <v>1</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <v>1</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="4">
         <v>5</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="4">
         <v>5</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="4">
         <v>5</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="4">
         <v>5</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="4">
         <v>5</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="4">
         <v>5</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="4">
@@ -1196,19 +1197,19 @@
       <c r="E20" s="4">
         <v>-1.821E-2</v>
       </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="4">
@@ -1217,19 +1218,19 @@
       <c r="E21" s="4">
         <v>-1.821E-2</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="6"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="4">
@@ -1238,19 +1239,19 @@
       <c r="E22" s="4">
         <v>-1.821E-2</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="4">
@@ -1259,19 +1260,19 @@
       <c r="E23" s="4">
         <v>-1.821E-2</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="4">
@@ -1280,19 +1281,19 @@
       <c r="E24" s="4">
         <v>-1.821E-2</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="4">
@@ -1301,19 +1302,19 @@
       <c r="E25" s="4">
         <v>-1.821E-2</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="6"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="4">
@@ -1322,19 +1323,19 @@
       <c r="E26" s="4">
         <v>-7.7499999999999999E-3</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="3"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="6"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="4">
@@ -1343,19 +1344,19 @@
       <c r="E27" s="4">
         <v>-7.7499999999999999E-3</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="6"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="4">
@@ -1364,19 +1365,19 @@
       <c r="E28" s="4">
         <v>-7.7499999999999999E-3</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="6"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D29" s="4">
@@ -1385,19 +1386,19 @@
       <c r="E29" s="4">
         <v>-7.7499999999999999E-3</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="6"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="4">
@@ -1406,19 +1407,19 @@
       <c r="E30" s="4">
         <v>-7.7499999999999999E-3</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="6"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D31" s="4">
@@ -1427,19 +1428,19 @@
       <c r="E31" s="4">
         <v>-7.7499999999999999E-3</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="6"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="4">
@@ -1448,19 +1449,19 @@
       <c r="E32" s="4">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="6"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="4">
@@ -1469,19 +1470,19 @@
       <c r="E33" s="4">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="6"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="4">
@@ -1490,19 +1491,19 @@
       <c r="E34" s="4">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="6"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="4">
@@ -1511,19 +1512,19 @@
       <c r="E35" s="4">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="6"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="4">
@@ -1532,19 +1533,19 @@
       <c r="E36" s="4">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="6"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="4">
@@ -1553,19 +1554,19 @@
       <c r="E37" s="4">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="6"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D38" s="4">
@@ -1574,19 +1575,19 @@
       <c r="E38" s="4">
         <v>-1.2999999999999999E-2</v>
       </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="6"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D39" s="4">
@@ -1595,19 +1596,19 @@
       <c r="E39" s="4">
         <v>-1.2999999999999999E-2</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="6"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D40" s="4">
@@ -1616,19 +1617,19 @@
       <c r="E40" s="4">
         <v>-1.2999999999999999E-2</v>
       </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="6"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D41" s="4">
@@ -1637,19 +1638,19 @@
       <c r="E41" s="4">
         <v>-1.2999999999999999E-2</v>
       </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="6"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="4">
@@ -1658,19 +1659,19 @@
       <c r="E42" s="4">
         <v>-1.2999999999999999E-2</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="6"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="4">
@@ -1679,19 +1680,19 @@
       <c r="E43" s="4">
         <v>-1.2999999999999999E-2</v>
       </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="6"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D44" s="4">
@@ -1700,19 +1701,19 @@
       <c r="E44" s="4">
         <v>-3.5000000000000001E-3</v>
       </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="6"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D45" s="4">
@@ -1721,19 +1722,19 @@
       <c r="E45" s="4">
         <v>-3.5000000000000001E-3</v>
       </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="6"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D46" s="4">
@@ -1742,19 +1743,19 @@
       <c r="E46" s="4">
         <v>-3.5000000000000001E-3</v>
       </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="6"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D47" s="4">
@@ -1763,19 +1764,19 @@
       <c r="E47" s="4">
         <v>-3.5000000000000001E-3</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="6"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="4">
@@ -1784,19 +1785,19 @@
       <c r="E48" s="4">
         <v>-3.5000000000000001E-3</v>
       </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="6"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D49" s="4">
@@ -1805,19 +1806,19 @@
       <c r="E49" s="4">
         <v>-3.5000000000000001E-3</v>
       </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="6"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D50" s="4">
@@ -1826,19 +1827,19 @@
       <c r="E50" s="4">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="F50" s="5"/>
-      <c r="G50" s="3"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="6"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D51" s="4">
@@ -1847,19 +1848,19 @@
       <c r="E51" s="4">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="6"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D52" s="4">
@@ -1868,19 +1869,19 @@
       <c r="E52" s="4">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="6"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D53" s="4">
@@ -1889,19 +1890,19 @@
       <c r="E53" s="4">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="F53" s="1"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="6"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="4">
@@ -1910,19 +1911,19 @@
       <c r="E54" s="4">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="F54" s="1"/>
-      <c r="G54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="6"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D55" s="4">
@@ -1931,19 +1932,19 @@
       <c r="E55" s="4">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="F55" s="1"/>
-      <c r="G55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="6"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="4">
@@ -1952,19 +1953,19 @@
       <c r="E56" s="4">
         <v>-8.2500000000000004E-3</v>
       </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="6"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D57" s="4">
@@ -1973,19 +1974,19 @@
       <c r="E57" s="4">
         <v>-8.2500000000000004E-3</v>
       </c>
-      <c r="F57" s="5"/>
-      <c r="G57" s="3"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="6"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D58" s="4">
@@ -1994,19 +1995,19 @@
       <c r="E58" s="4">
         <v>-8.2500000000000004E-3</v>
       </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="6"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D59" s="4">
@@ -2015,19 +2016,19 @@
       <c r="E59" s="4">
         <v>-8.2500000000000004E-3</v>
       </c>
-      <c r="F59" s="1"/>
-      <c r="G59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="6"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D60" s="4">
@@ -2036,19 +2037,19 @@
       <c r="E60" s="4">
         <v>-8.2500000000000004E-3</v>
       </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="6"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D61" s="4">
@@ -2057,19 +2058,19 @@
       <c r="E61" s="4">
         <v>-8.2500000000000004E-3</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="6"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D62" s="4">
@@ -2078,19 +2079,19 @@
       <c r="E62" s="4">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="F62" s="5"/>
-      <c r="G62" s="3"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="6"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D63" s="4">
@@ -2099,19 +2100,19 @@
       <c r="E63" s="4">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="6"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D64" s="4">
@@ -2120,19 +2121,19 @@
       <c r="E64" s="4">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="F64" s="1"/>
-      <c r="G64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="6"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="1:9">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D65" s="4">
@@ -2141,19 +2142,19 @@
       <c r="E65" s="4">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="F65" s="1"/>
-      <c r="G65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="6"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D66" s="4">
@@ -2162,19 +2163,19 @@
       <c r="E66" s="4">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="F66" s="1"/>
-      <c r="G66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="6"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D67" s="4">
@@ -2183,19 +2184,19 @@
       <c r="E67" s="4">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="F67" s="1"/>
-      <c r="G67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="6"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
     </row>
     <row r="68" spans="1:9">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D68" s="4">
@@ -2204,19 +2205,19 @@
       <c r="E68" s="4">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="F68" s="5"/>
-      <c r="G68" s="3"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="6"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D69" s="4">
@@ -2225,19 +2226,19 @@
       <c r="E69" s="4">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="F69" s="1"/>
-      <c r="G69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="6"/>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D70" s="4">
@@ -2246,19 +2247,19 @@
       <c r="E70" s="4">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="F70" s="1"/>
-      <c r="G70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="6"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D71" s="4">
@@ -2267,19 +2268,19 @@
       <c r="E71" s="4">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="F71" s="1"/>
-      <c r="G71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="6"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="1:9">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D72" s="4">
@@ -2288,19 +2289,19 @@
       <c r="E72" s="4">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="F72" s="1"/>
-      <c r="G72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="6"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D73" s="4">
@@ -2309,19 +2310,19 @@
       <c r="E73" s="4">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="F73" s="1"/>
-      <c r="G73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="6"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
     </row>
     <row r="74" spans="1:9">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D74" s="4">
@@ -2330,19 +2331,19 @@
       <c r="E74" s="4">
         <v>-2.0250000000000001E-2</v>
       </c>
-      <c r="F74" s="5"/>
-      <c r="G74" s="3"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="6"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
     </row>
     <row r="75" spans="1:9">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D75" s="4">
@@ -2351,19 +2352,19 @@
       <c r="E75" s="4">
         <v>-2.0250000000000001E-2</v>
       </c>
-      <c r="F75" s="1"/>
-      <c r="G75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="6"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
     </row>
     <row r="76" spans="1:9">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D76" s="4">
@@ -2372,19 +2373,19 @@
       <c r="E76" s="4">
         <v>-2.0250000000000001E-2</v>
       </c>
-      <c r="F76" s="1"/>
-      <c r="G76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="6"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
     </row>
     <row r="77" spans="1:9">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D77" s="4">
@@ -2393,19 +2394,19 @@
       <c r="E77" s="4">
         <v>-2.0250000000000001E-2</v>
       </c>
-      <c r="F77" s="1"/>
-      <c r="G77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="6"/>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
     </row>
     <row r="78" spans="1:9">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D78" s="4">
@@ -2414,19 +2415,19 @@
       <c r="E78" s="4">
         <v>-2.0250000000000001E-2</v>
       </c>
-      <c r="F78" s="1"/>
-      <c r="G78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="6"/>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
     </row>
     <row r="79" spans="1:9">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D79" s="4">
@@ -2435,19 +2436,19 @@
       <c r="E79" s="4">
         <v>-2.0250000000000001E-2</v>
       </c>
-      <c r="F79" s="1"/>
-      <c r="G79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="6"/>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D80" s="4">
@@ -2456,19 +2457,19 @@
       <c r="E80" s="4">
         <v>-1.6750000000000001E-2</v>
       </c>
-      <c r="F80" s="5"/>
-      <c r="G80" s="3"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="6"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
     </row>
     <row r="81" spans="1:9">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D81" s="4">
@@ -2477,19 +2478,19 @@
       <c r="E81" s="4">
         <v>-1.6750000000000001E-2</v>
       </c>
-      <c r="F81" s="1"/>
-      <c r="G81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="6"/>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D82" s="4">
@@ -2498,19 +2499,19 @@
       <c r="E82" s="4">
         <v>-1.6750000000000001E-2</v>
       </c>
-      <c r="F82" s="1"/>
-      <c r="G82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="6"/>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D83" s="4">
@@ -2519,19 +2520,19 @@
       <c r="E83" s="4">
         <v>-1.6750000000000001E-2</v>
       </c>
-      <c r="F83" s="1"/>
-      <c r="G83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="6"/>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
     </row>
     <row r="84" spans="1:9">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D84" s="4">
@@ -2540,19 +2541,19 @@
       <c r="E84" s="4">
         <v>-1.6750000000000001E-2</v>
       </c>
-      <c r="F84" s="1"/>
-      <c r="G84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="6"/>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="1:9">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D85" s="4">
@@ -2561,70 +2562,70 @@
       <c r="E85" s="4">
         <v>-1.6750000000000001E-2</v>
       </c>
-      <c r="F85" s="1"/>
-      <c r="G85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="6"/>
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="1:9">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C86" s="1"/>
+      <c r="C86" s="3"/>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
-      <c r="F86" s="7">
+      <c r="F86" s="5">
         <v>1</v>
       </c>
-      <c r="G86" s="3"/>
+      <c r="G86" s="6"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
     </row>
     <row r="87" spans="1:9">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C87" s="1"/>
+      <c r="C87" s="3"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
-      <c r="F87" s="7">
+      <c r="F87" s="5">
         <v>1</v>
       </c>
-      <c r="G87" s="3"/>
+      <c r="G87" s="6"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
     </row>
     <row r="88" spans="1:9">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C88" s="1"/>
+      <c r="C88" s="3"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
-      <c r="F88" s="7">
+      <c r="F88" s="5">
         <v>1</v>
       </c>
-      <c r="G88" s="3"/>
+      <c r="G88" s="6"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C89" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D89" s="4">
@@ -2633,19 +2634,19 @@
       <c r="E89" s="4">
         <v>-1.2E-2</v>
       </c>
-      <c r="F89" s="5"/>
-      <c r="G89" s="3"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="6"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="C90" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D90" s="4">
@@ -2654,19 +2655,19 @@
       <c r="E90" s="4">
         <v>-1.2E-2</v>
       </c>
-      <c r="F90" s="1"/>
-      <c r="G90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="6"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
     </row>
     <row r="91" spans="1:9">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C91" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D91" s="4">
@@ -2675,19 +2676,19 @@
       <c r="E91" s="4">
         <v>-1.2E-2</v>
       </c>
-      <c r="F91" s="1"/>
-      <c r="G91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="6"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="1" t="s">
+      <c r="A92" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D92" s="4">
@@ -2696,19 +2697,19 @@
       <c r="E92" s="4">
         <v>-1.2E-2</v>
       </c>
-      <c r="F92" s="1"/>
-      <c r="G92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="6"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
     </row>
     <row r="93" spans="1:9">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D93" s="4">
@@ -2717,19 +2718,19 @@
       <c r="E93" s="4">
         <v>-1.2E-2</v>
       </c>
-      <c r="F93" s="1"/>
-      <c r="G93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="6"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="1:9">
-      <c r="A94" s="1" t="s">
+      <c r="A94" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D94" s="4">
@@ -2738,65 +2739,65 @@
       <c r="E94" s="4">
         <v>-1.2E-2</v>
       </c>
-      <c r="F94" s="1"/>
-      <c r="G94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="6"/>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
     </row>
     <row r="95" spans="1:9">
-      <c r="A95" s="1" t="s">
+      <c r="A95" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C95" s="1"/>
+      <c r="C95" s="3"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
-      <c r="F95" s="7">
+      <c r="F95" s="5">
         <v>1</v>
       </c>
-      <c r="G95" s="3"/>
+      <c r="G95" s="6"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="1:9">
-      <c r="A96" s="1" t="s">
+      <c r="A96" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C96" s="1"/>
+      <c r="C96" s="3"/>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
-      <c r="F96" s="7">
+      <c r="F96" s="5">
         <v>1</v>
       </c>
-      <c r="G96" s="3"/>
+      <c r="G96" s="6"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
     </row>
     <row r="97" spans="1:9">
-      <c r="A97" s="1" t="s">
+      <c r="A97" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C97" s="1"/>
+      <c r="C97" s="3"/>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
-      <c r="F97" s="7">
+      <c r="F97" s="5">
         <v>1</v>
       </c>
-      <c r="G97" s="3"/>
+      <c r="G97" s="6"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>